<commit_message>
Fixed fish look-up file, and changed UI to receive input for its file path.
</commit_message>
<xml_diff>
--- a/fish_anadromy.xlsx
+++ b/fish_anadromy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\Google Drive\School\UW Bothell\CSS 383\Bioinformatics Team\Project 1\Python Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DADCE9A-4BC4-4FD6-9822-5327FDECE126}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74FE4F4-4ADE-42DE-BA3C-ED0B364ED3E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{AB1B2B8B-A255-44C0-9827-C98F6C00537A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB1B2B8B-A255-44C0-9827-C98F6C00537A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Common Name</t>
   </si>
@@ -81,22 +81,28 @@
     <t>Rainbow Trout</t>
   </si>
   <si>
-    <t>BCF660-07|Oncorhynchus_kisutch|COI-5P|EU524216</t>
-  </si>
-  <si>
-    <t>BCF447-07|Oncorhynchus_nerka|COI-5P|EU524226</t>
-  </si>
-  <si>
-    <t>ANGBF1310-12|Salvelinus_alpinus|COI-5P|HQ167686</t>
-  </si>
-  <si>
-    <t>ANGBF1309-12|Salmo_salar|COI-5P|HQ167685</t>
-  </si>
-  <si>
-    <t>ACLB015-06|Oncorhynchus_tshawytscha|COI-5P|HM102306</t>
-  </si>
-  <si>
-    <t>SDP15007-13|Oncorhynchus_mykiss|COI-5P|KJ592723</t>
+    <t>Salvelinus_alpinus|COI</t>
+  </si>
+  <si>
+    <t>Oncorhynchus_nerka|COI</t>
+  </si>
+  <si>
+    <t>Oncorhynchus_kisutch|COI</t>
+  </si>
+  <si>
+    <t>Steelhead Trout</t>
+  </si>
+  <si>
+    <t>Oncorhynchus_mykiss_steelhead_trout|COI</t>
+  </si>
+  <si>
+    <t>Oncorhynchus_mykiss_rainbow_trout|COI</t>
+  </si>
+  <si>
+    <t>Salmo_salar|COI</t>
+  </si>
+  <si>
+    <t>Oncorhynchus_tshawytscha|COI</t>
   </si>
 </sst>
 </file>
@@ -120,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -143,16 +149,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -469,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C16C670-ECDF-4B6E-8A2D-99EBBD1A2D2E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +522,7 @@
     </row>
     <row r="2" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -511,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -525,9 +548,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -555,7 +578,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -567,9 +590,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -579,6 +602,20 @@
       </c>
       <c r="D7" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>